<commit_message>
did the assignment for meta analysis
</commit_message>
<xml_diff>
--- a/13. Metaanalysis/data/metaanalysis_data.xlsx
+++ b/13. Metaanalysis/data/metaanalysis_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whardy\Desktop\RRCourse2023\13. Metaanalysis\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4703448c7c36860e/Desktop/RRcourse/RRcourse2023/13. Metaanalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2DE4F6-0204-4F07-BD8A-1DB7D972A2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{FA2DE4F6-0204-4F07-BD8A-1DB7D972A2C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCA011E5-6DE5-43C2-939C-33E8DD7E0BD3}"/>
   <bookViews>
-    <workbookView xWindow="6735" yWindow="2490" windowWidth="21600" windowHeight="11385" xr2:uid="{3C303B16-1778-4040-9FE8-FE3707D84BAD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3C303B16-1778-4040-9FE8-FE3707D84BAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz2" sheetId="2" r:id="rId1"/>
@@ -553,13 +553,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{126B0D72-E236-4C3B-A3F8-91C0ED779F39}">
   <dimension ref="A1:AB28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -645,7 +648,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -731,7 +734,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -817,7 +820,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -903,7 +906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -989,7 +992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1075,7 +1078,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -1161,7 +1164,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>18</v>
       </c>
@@ -1331,7 +1334,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1503,7 +1506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1589,7 +1592,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1675,7 +1678,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1761,7 +1764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1847,7 +1850,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -2019,7 +2022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -2105,7 +2108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -2191,7 +2194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2449,7 +2452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>11</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -2707,7 +2710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>11</v>
       </c>
@@ -2793,7 +2796,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -2879,7 +2882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>